<commit_message>
bitcoin auto trade with AI
</commit_message>
<xml_diff>
--- a/dd.xlsx
+++ b/dd.xlsx
@@ -498,28 +498,28 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44562.375</v>
+        <v>44566.375</v>
       </c>
       <c r="B2" t="n">
-        <v>56784000</v>
+        <v>56023000</v>
       </c>
       <c r="C2" t="n">
-        <v>58271000</v>
+        <v>57100000</v>
       </c>
       <c r="D2" t="n">
-        <v>56762000</v>
+        <v>52701000</v>
       </c>
       <c r="E2" t="n">
-        <v>57915000</v>
+        <v>53854000</v>
       </c>
       <c r="F2" t="n">
-        <v>2628.14596492</v>
+        <v>9296.798713509999</v>
       </c>
       <c r="G2" t="n">
-        <v>151064521830.3326</v>
+        <v>515276777193.213</v>
       </c>
       <c r="H2" t="n">
-        <v>754500</v>
+        <v>2199500</v>
       </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="n">
@@ -534,31 +534,31 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44563.375</v>
+        <v>44567.375</v>
       </c>
       <c r="B3" t="n">
-        <v>57915000</v>
+        <v>53854000</v>
       </c>
       <c r="C3" t="n">
-        <v>58300000</v>
+        <v>54300000</v>
       </c>
       <c r="D3" t="n">
-        <v>57100000</v>
+        <v>52388000</v>
       </c>
       <c r="E3" t="n">
-        <v>57531000</v>
+        <v>53239000</v>
       </c>
       <c r="F3" t="n">
-        <v>3567.5057124</v>
+        <v>6389.07930239</v>
       </c>
       <c r="G3" t="n">
-        <v>205291308789.9393</v>
+        <v>339630997052.0713</v>
       </c>
       <c r="H3" t="n">
-        <v>600000</v>
+        <v>956000</v>
       </c>
       <c r="I3" t="n">
-        <v>58669500</v>
+        <v>56053500</v>
       </c>
       <c r="J3" t="n">
         <v>2</v>
@@ -572,31 +572,31 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44564.375</v>
+        <v>44568.375</v>
       </c>
       <c r="B4" t="n">
-        <v>57540000</v>
+        <v>53240000</v>
       </c>
       <c r="C4" t="n">
-        <v>57749000</v>
+        <v>53358000</v>
       </c>
       <c r="D4" t="n">
-        <v>56133000</v>
+        <v>50900000</v>
       </c>
       <c r="E4" t="n">
-        <v>56641000</v>
+        <v>51449000</v>
       </c>
       <c r="F4" t="n">
-        <v>6304.95856401</v>
+        <v>7509.10809323</v>
       </c>
       <c r="G4" t="n">
-        <v>360063461140.0126</v>
+        <v>389528045895.4946</v>
       </c>
       <c r="H4" t="n">
-        <v>808000</v>
+        <v>1229000</v>
       </c>
       <c r="I4" t="n">
-        <v>58140000</v>
+        <v>54196000</v>
       </c>
       <c r="J4" t="n">
         <v>2</v>
@@ -610,113 +610,113 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44565.375</v>
+        <v>44569.375</v>
       </c>
       <c r="B5" t="n">
-        <v>56640000</v>
+        <v>51449000</v>
       </c>
       <c r="C5" t="n">
-        <v>57685000</v>
+        <v>52709000</v>
       </c>
       <c r="D5" t="n">
-        <v>56000000</v>
+        <v>50829000</v>
       </c>
       <c r="E5" t="n">
-        <v>56023000</v>
+        <v>52142000</v>
       </c>
       <c r="F5" t="n">
-        <v>6053.44580235</v>
+        <v>4171.09645762</v>
       </c>
       <c r="G5" t="n">
-        <v>342512644132.8362</v>
+        <v>215423691964.9106</v>
       </c>
       <c r="H5" t="n">
-        <v>842500</v>
+        <v>940000</v>
       </c>
       <c r="I5" t="n">
-        <v>57448000</v>
+        <v>52678000</v>
       </c>
       <c r="J5" t="n">
-        <v>0.9751949589193706</v>
+        <v>0.9398249743726034</v>
       </c>
       <c r="K5" t="n">
-        <v>7.801559671354965</v>
+        <v>7.518599794980827</v>
       </c>
       <c r="L5" t="n">
-        <v>2.480504108062942</v>
+        <v>6.017502562739663</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44566.375</v>
+        <v>44570.375</v>
       </c>
       <c r="B6" t="n">
-        <v>56023000</v>
+        <v>52142000</v>
       </c>
       <c r="C6" t="n">
-        <v>57100000</v>
+        <v>52600000</v>
       </c>
       <c r="D6" t="n">
-        <v>52701000</v>
+        <v>51144000</v>
       </c>
       <c r="E6" t="n">
-        <v>53854000</v>
+        <v>51678000</v>
       </c>
       <c r="F6" t="n">
-        <v>9296.798713509999</v>
+        <v>3369.09508974</v>
       </c>
       <c r="G6" t="n">
-        <v>515276777193.213</v>
+        <v>174869889802.5734</v>
       </c>
       <c r="H6" t="n">
-        <v>2199500</v>
+        <v>728000</v>
       </c>
       <c r="I6" t="n">
-        <v>56865500</v>
+        <v>53082000</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9470417036691843</v>
+        <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>7.388402362436807</v>
+        <v>15.03719958996165</v>
       </c>
       <c r="L6" t="n">
-        <v>7.644970469539913</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44567.375</v>
+        <v>44571.375</v>
       </c>
       <c r="B7" t="n">
-        <v>53854000</v>
+        <v>51672000</v>
       </c>
       <c r="C7" t="n">
-        <v>54300000</v>
+        <v>51999000</v>
       </c>
       <c r="D7" t="n">
-        <v>52388000</v>
+        <v>48897000</v>
       </c>
       <c r="E7" t="n">
-        <v>53239000</v>
+        <v>51246000</v>
       </c>
       <c r="F7" t="n">
-        <v>6389.07930239</v>
+        <v>7955.46011133</v>
       </c>
       <c r="G7" t="n">
-        <v>339630997052.0713</v>
+        <v>402570820215.6586</v>
       </c>
       <c r="H7" t="n">
-        <v>956000</v>
+        <v>1551000</v>
       </c>
       <c r="I7" t="n">
-        <v>56053500</v>
+        <v>52400000</v>
       </c>
       <c r="J7" t="n">
         <v>2</v>
       </c>
       <c r="K7" t="n">
-        <v>14.77680472487361</v>
+        <v>30.07439917992331</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
@@ -724,37 +724,37 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44568.375</v>
+        <v>44572.375</v>
       </c>
       <c r="B8" t="n">
-        <v>53240000</v>
+        <v>51255000</v>
       </c>
       <c r="C8" t="n">
-        <v>53358000</v>
+        <v>51699000</v>
       </c>
       <c r="D8" t="n">
-        <v>50900000</v>
+        <v>50680000</v>
       </c>
       <c r="E8" t="n">
-        <v>51695000</v>
+        <v>51169000</v>
       </c>
       <c r="F8" t="n">
-        <v>6174.15369409</v>
+        <v>3402.34941034</v>
       </c>
       <c r="G8" t="n">
-        <v>320808214326.8934</v>
+        <v>174173355966.096</v>
       </c>
       <c r="H8" t="n">
-        <v>1229000</v>
+        <v>509500</v>
       </c>
       <c r="I8" t="n">
-        <v>54196000</v>
+        <v>52806000</v>
       </c>
       <c r="J8" t="n">
         <v>2</v>
       </c>
       <c r="K8" t="n">
-        <v>29.55360944974723</v>
+        <v>60.14879835984662</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>

</xml_diff>